<commit_message>
got basic demo working
</commit_message>
<xml_diff>
--- a/headcount_summary.xlsx
+++ b/headcount_summary.xlsx
@@ -15,9 +15,9 @@
     <sheet name="monthly_headcount_summary" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">monthly_headcount_summary!$A$1:$E$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">monthly_headcount_summary!$A$1:$G$53</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="84">
   <si>
     <t>division</t>
   </si>
@@ -62,63 +62,36 @@
     <t>52P02</t>
   </si>
   <si>
-    <t>Employee_1</t>
-  </si>
-  <si>
     <t>dirsa</t>
   </si>
   <si>
     <t>52P10</t>
   </si>
   <si>
-    <t>Employee_2</t>
-  </si>
-  <si>
     <t>55335</t>
   </si>
   <si>
-    <t>Employee_3</t>
-  </si>
-  <si>
     <t>ffirs</t>
   </si>
   <si>
     <t>52P04</t>
   </si>
   <si>
-    <t>Employee_4</t>
-  </si>
-  <si>
     <t>55308</t>
   </si>
   <si>
-    <t>Employee_5</t>
-  </si>
-  <si>
     <t>nahan</t>
   </si>
   <si>
     <t>61101</t>
   </si>
   <si>
-    <t>Employee_6</t>
-  </si>
-  <si>
     <t>nzali</t>
   </si>
   <si>
-    <t>Employee_7</t>
-  </si>
-  <si>
     <t>52P01</t>
   </si>
   <si>
-    <t>Employee_8</t>
-  </si>
-  <si>
-    <t>Employee_9</t>
-  </si>
-  <si>
     <t>Employee_10</t>
   </si>
   <si>
@@ -263,9 +236,6 @@
     <t>Employee_47</t>
   </si>
   <si>
-    <t>2000</t>
-  </si>
-  <si>
     <t>57100</t>
   </si>
   <si>
@@ -288,15 +258,58 @@
   </si>
   <si>
     <t>Employee_52</t>
+  </si>
+  <si>
+    <t>Employee_01</t>
+  </si>
+  <si>
+    <t>Employee_02</t>
+  </si>
+  <si>
+    <t>Employee_03</t>
+  </si>
+  <si>
+    <t>Employee_04</t>
+  </si>
+  <si>
+    <t>Employee_05</t>
+  </si>
+  <si>
+    <t>Employee_06</t>
+  </si>
+  <si>
+    <t>Employee_07</t>
+  </si>
+  <si>
+    <t>Employee_08</t>
+  </si>
+  <si>
+    <t>Employee_09</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -319,14 +332,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -605,7 +622,7 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -653,16 +670,16 @@
         <v>899591</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -670,22 +687,22 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>811272</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="G3">
-        <v>108</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -693,22 +710,22 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>810761</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F4">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="G4">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
@@ -716,22 +733,22 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>1098762</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5">
-        <v>46</v>
+        <v>156</v>
       </c>
       <c r="G5">
-        <v>114</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
@@ -739,22 +756,22 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>897932</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F6">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G6">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
@@ -762,22 +779,22 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>814863</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7">
-        <v>11</v>
-      </c>
-      <c r="G7">
-        <v>149</v>
+        <v>17</v>
+      </c>
+      <c r="F7" s="1">
+        <v>60</v>
+      </c>
+      <c r="G7" s="1">
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
@@ -785,22 +802,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>820239</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F8">
-        <v>107</v>
+        <v>46</v>
       </c>
       <c r="G8">
-        <v>53</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
@@ -808,22 +825,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>832272</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="G9">
-        <v>134</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
@@ -837,16 +854,16 @@
         <v>825881</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G10">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
@@ -854,22 +871,22 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>906780</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G11">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
@@ -877,22 +894,22 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>1081500</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="G12">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
@@ -900,22 +917,22 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C13">
         <v>1090593</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="G13">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
@@ -923,22 +940,22 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>820001</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14">
-        <v>156</v>
+        <v>46</v>
       </c>
       <c r="G14">
-        <v>4</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
@@ -946,22 +963,22 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C15">
         <v>1099812</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="G15">
-        <v>96</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
@@ -969,22 +986,22 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>826917</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="G16">
-        <v>114</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
@@ -992,22 +1009,22 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C17">
         <v>1101478</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G17">
-        <v>148</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
@@ -1015,22 +1032,22 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C18">
         <v>1098279</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G18">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
@@ -1038,22 +1055,22 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C19">
         <v>826924</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19">
-        <v>73</v>
+        <v>112</v>
       </c>
       <c r="G19">
-        <v>87</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
@@ -1061,22 +1078,22 @@
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C20">
         <v>801836</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F20">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="G20">
-        <v>64</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
@@ -1084,22 +1101,22 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C21">
         <v>1100974</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="F21">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
@@ -1107,22 +1124,22 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C22">
         <v>1099700</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="G22">
-        <v>117</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
@@ -1130,22 +1147,22 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C23">
         <v>1075893</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23">
-        <v>79</v>
+        <v>146</v>
       </c>
       <c r="G23">
-        <v>81</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.15">
@@ -1153,22 +1170,22 @@
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C24">
         <v>801717</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E24" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F24">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="G24">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
@@ -1176,22 +1193,22 @@
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C25">
         <v>894901</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25">
-        <v>130</v>
+        <v>73</v>
       </c>
       <c r="G25">
-        <v>30</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">
@@ -1199,22 +1216,22 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C26">
         <v>1078455</v>
       </c>
       <c r="D26" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G26">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.15">
@@ -1222,22 +1239,22 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C27">
         <v>810425</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E27" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F27">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="G27">
-        <v>40</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.15">
@@ -1245,22 +1262,22 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C28">
         <v>849079</v>
       </c>
       <c r="D28" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="G28">
-        <v>88</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.15">
@@ -1268,22 +1285,22 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C29">
         <v>1079484</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E29" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="F29">
-        <v>37</v>
+        <v>114</v>
       </c>
       <c r="G29">
-        <v>123</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.15">
@@ -1291,22 +1308,22 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C30">
         <v>806974</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F30">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="G30">
-        <v>67</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.15">
@@ -1314,22 +1331,22 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C31">
         <v>826693</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="G31">
-        <v>99</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.15">
@@ -1337,22 +1354,22 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C32">
         <v>899913</v>
       </c>
       <c r="D32" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="G32">
-        <v>44</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.15">
@@ -1360,22 +1377,22 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C33">
         <v>806092</v>
       </c>
       <c r="D33" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E33" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F33">
+        <v>46</v>
+      </c>
+      <c r="G33">
         <v>114</v>
-      </c>
-      <c r="G33">
-        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.15">
@@ -1383,22 +1400,22 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C34">
         <v>897869</v>
       </c>
       <c r="D34" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34">
-        <v>55</v>
+        <v>128</v>
       </c>
       <c r="G34">
-        <v>105</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.15">
@@ -1406,22 +1423,22 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C35">
         <v>811216</v>
       </c>
       <c r="D35" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35">
-        <v>140</v>
+        <v>11</v>
       </c>
       <c r="G35">
-        <v>20</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.15">
@@ -1429,22 +1446,22 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C36">
         <v>830291</v>
       </c>
       <c r="D36" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F36">
-        <v>99</v>
+        <v>159</v>
       </c>
       <c r="G36">
-        <v>61</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.15">
@@ -1452,22 +1469,22 @@
         <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C37">
         <v>1074010</v>
       </c>
       <c r="D37" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E37" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="F37">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G37">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.15">
@@ -1475,22 +1492,22 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C38">
         <v>849758</v>
       </c>
       <c r="D38" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38">
-        <v>158</v>
+        <v>116</v>
       </c>
       <c r="G38">
-        <v>2</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.15">
@@ -1498,22 +1515,22 @@
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C39">
         <v>1083873</v>
       </c>
       <c r="D39" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E39" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="F39">
-        <v>84</v>
+        <v>140</v>
       </c>
       <c r="G39">
-        <v>76</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.15">
@@ -1521,22 +1538,22 @@
         <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C40">
         <v>831075</v>
       </c>
       <c r="D40" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F40">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G40">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.15">
@@ -1544,22 +1561,22 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C41">
         <v>849380</v>
       </c>
       <c r="D41" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E41" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="F41">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="G41">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.15">
@@ -1567,22 +1584,22 @@
         <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C42">
         <v>1063013</v>
       </c>
       <c r="D42" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="G42">
-        <v>37</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.15">
@@ -1590,22 +1607,22 @@
         <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C43">
         <v>807275</v>
       </c>
       <c r="D43" t="s">
+        <v>61</v>
+      </c>
+      <c r="E43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43">
+        <v>90</v>
+      </c>
+      <c r="G43">
         <v>70</v>
-      </c>
-      <c r="E43" t="s">
-        <v>15</v>
-      </c>
-      <c r="F43">
-        <v>8</v>
-      </c>
-      <c r="G43">
-        <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.15">
@@ -1613,22 +1630,22 @@
         <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C44">
         <v>821100</v>
       </c>
       <c r="D44" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F44">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G44">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.15">
@@ -1636,22 +1653,22 @@
         <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C45">
         <v>815346</v>
       </c>
       <c r="D45" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45">
-        <v>144</v>
+        <v>26</v>
       </c>
       <c r="G45">
-        <v>16</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.15">
@@ -1659,22 +1676,22 @@
         <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C46">
         <v>806771</v>
       </c>
       <c r="D46" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F46">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G46">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.15">
@@ -1682,22 +1699,22 @@
         <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C47">
         <v>820596</v>
       </c>
       <c r="D47" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47">
-        <v>121</v>
+        <v>89</v>
       </c>
       <c r="G47">
-        <v>39</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.15">
@@ -1705,45 +1722,45 @@
         <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C48">
         <v>1102073</v>
       </c>
       <c r="D48" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F48">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G48">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C49">
         <v>841596</v>
       </c>
       <c r="D49" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E49" t="s">
-        <v>79</v>
-      </c>
-      <c r="F49">
-        <v>38</v>
-      </c>
-      <c r="G49">
-        <v>122</v>
+        <v>69</v>
+      </c>
+      <c r="F49" s="1">
+        <v>46</v>
+      </c>
+      <c r="G49" s="1">
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.15">
@@ -1751,68 +1768,68 @@
         <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C50">
         <v>1106301</v>
       </c>
       <c r="D50" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="G50">
-        <v>114</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A51" s="1" t="s">
-        <v>76</v>
+      <c r="A51" t="s">
+        <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C51" s="1">
         <v>1206301</v>
       </c>
       <c r="D51" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F51" s="1">
-        <v>46</v>
-      </c>
-      <c r="G51" s="1">
-        <v>114</v>
+        <v>69</v>
+      </c>
+      <c r="F51">
+        <v>21</v>
+      </c>
+      <c r="G51">
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A52" s="1" t="s">
-        <v>76</v>
+      <c r="A52" t="s">
+        <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C52" s="1">
         <v>1206302</v>
       </c>
       <c r="D52" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="E52" t="s">
-        <v>43</v>
-      </c>
-      <c r="F52" s="1">
-        <v>60</v>
-      </c>
-      <c r="G52" s="1">
-        <v>100</v>
+        <v>34</v>
+      </c>
+      <c r="F52">
+        <v>52</v>
+      </c>
+      <c r="G52">
+        <v>108</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.15">
@@ -1820,26 +1837,33 @@
         <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C53" s="1">
         <v>1206303</v>
       </c>
       <c r="D53" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="E53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="G53">
-        <v>114</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E53"/>
+  <autoFilter ref="A1:G53">
+    <sortState ref="A2:G53">
+      <sortCondition ref="D1:D53"/>
+    </sortState>
+  </autoFilter>
+  <sortState ref="A2:G53">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>

</xml_diff>

<commit_message>
spreadsheet files updated on recompute
</commit_message>
<xml_diff>
--- a/headcount_summary.xlsx
+++ b/headcount_summary.xlsx
@@ -622,7 +622,7 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection sqref="A1:G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1856,11 +1856,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G53">
-    <sortState ref="A2:G53">
-      <sortCondition ref="D1:D53"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:G53"/>
   <sortState ref="A2:G53">
     <sortCondition ref="A1"/>
   </sortState>

</xml_diff>